<commit_message>
Additional updates to frame. Established durations should be [start_duration, end_duration) for inclusion.
</commit_message>
<xml_diff>
--- a/tests/model_tools/data/frame-examples.xlsx
+++ b/tests/model_tools/data/frame-examples.xlsx
@@ -21,9 +21,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="20">
-  <si>
-    <t xml:space="preserve">Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="24">
+  <si>
+    <t xml:space="preserve">Test Month Duration</t>
   </si>
   <si>
     <t xml:space="preserve">start_dt</t>
@@ -41,19 +41,31 @@
     <t xml:space="preserve">col_date_nm</t>
   </si>
   <si>
+    <t xml:space="preserve">date_bd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end_duration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_ed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">duration_month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">duration_quarter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">duration_year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Month Calendar</t>
+  </si>
+  <si>
     <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">duration_month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">duration_quarter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">duration_year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Return</t>
   </si>
   <si>
     <t xml:space="preserve">calendar_year</t>
@@ -89,7 +101,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -316,36 +328,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:E46"/>
+  <dimension ref="B1:F47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="4" t="s">
@@ -384,533 +397,638 @@
         <v>7</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="B11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="7" t="s">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="11" t="n">
-        <v>43840</v>
-      </c>
-      <c r="C17" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C17-1)/3)+1</f>
-        <v>1</v>
-      </c>
-      <c r="E17" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C17-1)/12)+1</f>
-        <v>1</v>
+      <c r="F17" s="10" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="11" t="n">
+        <v>43840</v>
+      </c>
+      <c r="C18" s="11" t="n">
         <v>43871</v>
       </c>
-      <c r="C18" s="1" t="n">
-        <v>2</v>
-      </c>
       <c r="D18" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C18-1)/3)+1</f>
         <v>1</v>
       </c>
       <c r="E18" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C18-1)/12)+1</f>
+        <f aca="false">_xlfn.FLOOR.MATH((D18-1)/3)+1</f>
+        <v>1</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D18-1)/12)+1</f>
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="11" t="n">
+        <v>43871</v>
+      </c>
+      <c r="C19" s="11" t="n">
         <v>43900</v>
       </c>
-      <c r="C19" s="1" t="n">
-        <v>3</v>
-      </c>
       <c r="D19" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C19-1)/3)+1</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C19-1)/12)+1</f>
+        <f aca="false">_xlfn.FLOOR.MATH((D19-1)/3)+1</f>
+        <v>1</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D19-1)/12)+1</f>
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="11" t="n">
+        <v>43900</v>
+      </c>
+      <c r="C20" s="11" t="n">
         <v>43931</v>
       </c>
-      <c r="C20" s="1" t="n">
-        <v>4</v>
-      </c>
       <c r="D20" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C20-1)/3)+1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C20-1)/12)+1</f>
+        <f aca="false">_xlfn.FLOOR.MATH((D20-1)/3)+1</f>
+        <v>1</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D20-1)/12)+1</f>
         <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="11" t="n">
+        <v>43931</v>
+      </c>
+      <c r="C21" s="11" t="n">
         <v>43961</v>
       </c>
-      <c r="C21" s="1" t="n">
-        <v>5</v>
-      </c>
       <c r="D21" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C21-1)/3)+1</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E21" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C21-1)/12)+1</f>
+        <f aca="false">_xlfn.FLOOR.MATH((D21-1)/3)+1</f>
+        <v>2</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D21-1)/12)+1</f>
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="11" t="n">
+        <v>43961</v>
+      </c>
+      <c r="C22" s="11" t="n">
         <v>43992</v>
       </c>
-      <c r="C22" s="1" t="n">
-        <v>6</v>
-      </c>
       <c r="D22" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C22-1)/3)+1</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E22" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C22-1)/12)+1</f>
+        <f aca="false">_xlfn.FLOOR.MATH((D22-1)/3)+1</f>
+        <v>2</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D22-1)/12)+1</f>
         <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="11" t="n">
+        <v>43992</v>
+      </c>
+      <c r="C23" s="11" t="n">
         <v>44022</v>
       </c>
-      <c r="C23" s="1" t="n">
-        <v>7</v>
-      </c>
       <c r="D23" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C23-1)/3)+1</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E23" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C23-1)/12)+1</f>
+        <f aca="false">_xlfn.FLOOR.MATH((D23-1)/3)+1</f>
+        <v>2</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D23-1)/12)+1</f>
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="11" t="n">
+        <v>44022</v>
+      </c>
+      <c r="C24" s="11" t="n">
         <v>44053</v>
       </c>
-      <c r="C24" s="1" t="n">
-        <v>8</v>
-      </c>
       <c r="D24" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C24-1)/3)+1</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E24" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C24-1)/12)+1</f>
+        <f aca="false">_xlfn.FLOOR.MATH((D24-1)/3)+1</f>
+        <v>3</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D24-1)/12)+1</f>
         <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="11" t="n">
+        <v>44053</v>
+      </c>
+      <c r="C25" s="11" t="n">
         <v>44084</v>
       </c>
-      <c r="C25" s="1" t="n">
-        <v>9</v>
-      </c>
       <c r="D25" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C25-1)/3)+1</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E25" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C25-1)/12)+1</f>
+        <f aca="false">_xlfn.FLOOR.MATH((D25-1)/3)+1</f>
+        <v>3</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D25-1)/12)+1</f>
         <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="11" t="n">
+        <v>44084</v>
+      </c>
+      <c r="C26" s="11" t="n">
         <v>44114</v>
       </c>
-      <c r="C26" s="1" t="n">
-        <v>10</v>
-      </c>
       <c r="D26" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C26-1)/3)+1</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E26" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C26-1)/12)+1</f>
+        <f aca="false">_xlfn.FLOOR.MATH((D26-1)/3)+1</f>
+        <v>3</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D26-1)/12)+1</f>
         <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="11" t="n">
+        <v>44114</v>
+      </c>
+      <c r="C27" s="11" t="n">
         <v>44145</v>
       </c>
-      <c r="C27" s="1" t="n">
-        <v>11</v>
-      </c>
       <c r="D27" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C27-1)/3)+1</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E27" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C27-1)/12)+1</f>
+        <f aca="false">_xlfn.FLOOR.MATH((D27-1)/3)+1</f>
+        <v>4</v>
+      </c>
+      <c r="F27" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D27-1)/12)+1</f>
         <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="11" t="n">
+        <v>44145</v>
+      </c>
+      <c r="C28" s="11" t="n">
         <v>44175</v>
       </c>
-      <c r="C28" s="1" t="n">
-        <v>12</v>
-      </c>
       <c r="D28" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C28-1)/3)+1</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E28" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C28-1)/12)+1</f>
+        <f aca="false">_xlfn.FLOOR.MATH((D28-1)/3)+1</f>
+        <v>4</v>
+      </c>
+      <c r="F28" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D28-1)/12)+1</f>
         <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="11" t="n">
+        <v>44175</v>
+      </c>
+      <c r="C29" s="11" t="n">
         <v>44206</v>
       </c>
-      <c r="C29" s="1" t="n">
-        <v>13</v>
-      </c>
       <c r="D29" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C29-1)/3)+1</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E29" s="1" t="n">
-        <v>2</v>
+        <f aca="false">_xlfn.FLOOR.MATH((D29-1)/3)+1</f>
+        <v>4</v>
+      </c>
+      <c r="F29" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D29-1)/12)+1</f>
+        <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="11" t="n">
+        <v>44206</v>
+      </c>
+      <c r="C30" s="11" t="n">
         <v>44237</v>
       </c>
-      <c r="C30" s="1" t="n">
-        <v>14</v>
-      </c>
       <c r="D30" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C30-1)/3)+1</f>
+        <v>13</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D30-1)/3)+1</f>
         <v>5</v>
       </c>
-      <c r="E30" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C30-1)/12)+1</f>
+      <c r="F30" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="11" t="n">
+        <v>44237</v>
+      </c>
+      <c r="C31" s="11" t="n">
         <v>44265</v>
       </c>
-      <c r="C31" s="1" t="n">
-        <v>15</v>
-      </c>
       <c r="D31" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C31-1)/3)+1</f>
+        <v>14</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D31-1)/3)+1</f>
         <v>5</v>
       </c>
-      <c r="E31" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C31-1)/12)+1</f>
+      <c r="F31" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D31-1)/12)+1</f>
         <v>2</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="11" t="n">
+        <v>44265</v>
+      </c>
+      <c r="C32" s="11" t="n">
         <v>44296</v>
       </c>
-      <c r="C32" s="1" t="n">
-        <v>16</v>
-      </c>
       <c r="D32" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C32-1)/3)+1</f>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E32" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C32-1)/12)+1</f>
+        <f aca="false">_xlfn.FLOOR.MATH((D32-1)/3)+1</f>
+        <v>5</v>
+      </c>
+      <c r="F32" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D32-1)/12)+1</f>
         <v>2</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="11" t="n">
+        <v>44296</v>
+      </c>
+      <c r="C33" s="11" t="n">
         <v>44326</v>
       </c>
-      <c r="C33" s="1" t="n">
-        <v>17</v>
-      </c>
       <c r="D33" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C33-1)/3)+1</f>
+        <v>16</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D33-1)/3)+1</f>
         <v>6</v>
       </c>
-      <c r="E33" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C33-1)/12)+1</f>
+      <c r="F33" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D33-1)/12)+1</f>
         <v>2</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="11" t="n">
+        <v>44326</v>
+      </c>
+      <c r="C34" s="11" t="n">
         <v>44357</v>
       </c>
-      <c r="C34" s="1" t="n">
-        <v>18</v>
-      </c>
       <c r="D34" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C34-1)/3)+1</f>
+        <v>17</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D34-1)/3)+1</f>
         <v>6</v>
       </c>
-      <c r="E34" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C34-1)/12)+1</f>
+      <c r="F34" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D34-1)/12)+1</f>
         <v>2</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="11" t="n">
+        <v>44357</v>
+      </c>
+      <c r="C35" s="11" t="n">
         <v>44387</v>
       </c>
-      <c r="C35" s="1" t="n">
-        <v>19</v>
-      </c>
       <c r="D35" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C35-1)/3)+1</f>
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E35" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C35-1)/12)+1</f>
+        <f aca="false">_xlfn.FLOOR.MATH((D35-1)/3)+1</f>
+        <v>6</v>
+      </c>
+      <c r="F35" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D35-1)/12)+1</f>
         <v>2</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="11" t="n">
+        <v>44387</v>
+      </c>
+      <c r="C36" s="11" t="n">
         <v>44418</v>
       </c>
-      <c r="C36" s="1" t="n">
-        <v>20</v>
-      </c>
       <c r="D36" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C36-1)/3)+1</f>
+        <v>19</v>
+      </c>
+      <c r="E36" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D36-1)/3)+1</f>
         <v>7</v>
       </c>
-      <c r="E36" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C36-1)/12)+1</f>
+      <c r="F36" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D36-1)/12)+1</f>
         <v>2</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="11" t="n">
+        <v>44418</v>
+      </c>
+      <c r="C37" s="11" t="n">
         <v>44449</v>
       </c>
-      <c r="C37" s="1" t="n">
-        <v>21</v>
-      </c>
       <c r="D37" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C37-1)/3)+1</f>
+        <v>20</v>
+      </c>
+      <c r="E37" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D37-1)/3)+1</f>
         <v>7</v>
       </c>
-      <c r="E37" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C37-1)/12)+1</f>
+      <c r="F37" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D37-1)/12)+1</f>
         <v>2</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="11" t="n">
+        <v>44449</v>
+      </c>
+      <c r="C38" s="11" t="n">
         <v>44479</v>
       </c>
-      <c r="C38" s="1" t="n">
-        <v>22</v>
-      </c>
       <c r="D38" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C38-1)/3)+1</f>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E38" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C38-1)/12)+1</f>
+        <f aca="false">_xlfn.FLOOR.MATH((D38-1)/3)+1</f>
+        <v>7</v>
+      </c>
+      <c r="F38" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D38-1)/12)+1</f>
         <v>2</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="11" t="n">
+        <v>44479</v>
+      </c>
+      <c r="C39" s="11" t="n">
         <v>44510</v>
       </c>
-      <c r="C39" s="1" t="n">
-        <v>23</v>
-      </c>
       <c r="D39" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C39-1)/3)+1</f>
+        <v>22</v>
+      </c>
+      <c r="E39" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D39-1)/3)+1</f>
         <v>8</v>
       </c>
-      <c r="E39" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C39-1)/12)+1</f>
+      <c r="F39" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D39-1)/12)+1</f>
         <v>2</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="11" t="n">
+        <v>44510</v>
+      </c>
+      <c r="C40" s="11" t="n">
         <v>44540</v>
       </c>
-      <c r="C40" s="1" t="n">
-        <v>24</v>
-      </c>
       <c r="D40" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C40-1)/3)+1</f>
+        <v>23</v>
+      </c>
+      <c r="E40" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D40-1)/3)+1</f>
         <v>8</v>
       </c>
-      <c r="E40" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C40-1)/12)+1</f>
+      <c r="F40" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D40-1)/12)+1</f>
         <v>2</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="11" t="n">
+        <v>44540</v>
+      </c>
+      <c r="C41" s="11" t="n">
         <v>44571</v>
       </c>
-      <c r="C41" s="1" t="n">
-        <v>25</v>
-      </c>
       <c r="D41" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C41-1)/3)+1</f>
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E41" s="1" t="n">
-        <v>3</v>
+        <f aca="false">_xlfn.FLOOR.MATH((D41-1)/3)+1</f>
+        <v>8</v>
+      </c>
+      <c r="F41" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D41-1)/12)+1</f>
+        <v>2</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="11" t="n">
+        <v>44571</v>
+      </c>
+      <c r="C42" s="11" t="n">
         <v>44602</v>
       </c>
-      <c r="C42" s="1" t="n">
-        <v>26</v>
-      </c>
       <c r="D42" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C42-1)/3)+1</f>
+        <v>25</v>
+      </c>
+      <c r="E42" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D42-1)/3)+1</f>
         <v>9</v>
       </c>
-      <c r="E42" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C42-1)/12)+1</f>
+      <c r="F42" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="11" t="n">
+        <v>44602</v>
+      </c>
+      <c r="C43" s="11" t="n">
         <v>44630</v>
       </c>
-      <c r="C43" s="1" t="n">
-        <v>27</v>
-      </c>
       <c r="D43" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C43-1)/3)+1</f>
+        <v>26</v>
+      </c>
+      <c r="E43" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D43-1)/3)+1</f>
         <v>9</v>
       </c>
-      <c r="E43" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C43-1)/12)+1</f>
+      <c r="F43" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D43-1)/12)+1</f>
         <v>3</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="11" t="n">
+        <v>44630</v>
+      </c>
+      <c r="C44" s="11" t="n">
         <v>44661</v>
       </c>
-      <c r="C44" s="1" t="n">
-        <v>28</v>
-      </c>
       <c r="D44" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C44-1)/3)+1</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E44" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C44-1)/12)+1</f>
+        <f aca="false">_xlfn.FLOOR.MATH((D44-1)/3)+1</f>
+        <v>9</v>
+      </c>
+      <c r="F44" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D44-1)/12)+1</f>
         <v>3</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="11" t="n">
+        <v>44661</v>
+      </c>
+      <c r="C45" s="11" t="n">
         <v>44691</v>
       </c>
-      <c r="C45" s="1" t="n">
-        <v>29</v>
-      </c>
       <c r="D45" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C45-1)/3)+1</f>
+        <v>28</v>
+      </c>
+      <c r="E45" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D45-1)/3)+1</f>
         <v>10</v>
       </c>
-      <c r="E45" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C45-1)/12)+1</f>
+      <c r="F45" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D45-1)/12)+1</f>
         <v>3</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="11" t="n">
+        <v>44691</v>
+      </c>
+      <c r="C46" s="11" t="n">
         <v>44722</v>
       </c>
-      <c r="C46" s="1" t="n">
+      <c r="D46" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="E46" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D46-1)/3)+1</f>
+        <v>10</v>
+      </c>
+      <c r="F46" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D46-1)/12)+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="11" t="n">
+        <v>44722</v>
+      </c>
+      <c r="C47" s="11" t="n">
+        <v>44752</v>
+      </c>
+      <c r="D47" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="D46" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C46-1)/3)+1</f>
+      <c r="E47" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D47-1)/3)+1</f>
         <v>10</v>
       </c>
-      <c r="E46" s="1" t="n">
-        <f aca="false">_xlfn.FLOOR.MATH((C46-1)/12)+1</f>
+      <c r="F47" s="1" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((D47-1)/12)+1</f>
         <v>3</v>
       </c>
     </row>
@@ -926,21 +1044,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="B1:L51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.02"/>
@@ -956,7 +1074,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="3" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -992,79 +1110,79 @@
         <v>5</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1077,7 +1195,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="9"/>
@@ -1095,34 +1213,34 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="10" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L22" s="0"/>
     </row>

</xml_diff>